<commit_message>
excel-report-template select by user id
</commit_message>
<xml_diff>
--- a/templates/export/summary.xlsx
+++ b/templates/export/summary.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4197F1C-5088-4B17-9B53-385EB58E96B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Автор</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]&quot; h &quot;m&quot; min&quot;"/>
   </numFmts>
@@ -249,12 +250,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -297,9 +292,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -399,7 +400,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -442,7 +449,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -735,11 +748,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,114 +766,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:9" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="15" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>